<commit_message>
edited the component list
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -69,15 +69,9 @@
     <t>11.8K</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
     <t>1.07K</t>
   </si>
   <si>
-    <t>5.62K</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>DF13</t>
+  </si>
+  <si>
+    <t>3.32K</t>
+  </si>
+  <si>
+    <t>61.9k</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
   </sheetPr>
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -792,7 +792,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
@@ -812,7 +812,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
@@ -830,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
@@ -848,7 +848,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
@@ -868,7 +868,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -888,7 +888,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
@@ -908,7 +908,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -928,7 +928,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -1057,10 +1057,10 @@
         <v>2</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>1</v>
@@ -1071,10 +1071,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D32" s="2">
         <v>1</v>
@@ -1085,10 +1085,10 @@
         <v>2</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D33" s="2">
         <v>2</v>
@@ -1099,10 +1099,10 @@
         <v>3</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D34" s="2">
         <v>1</v>
@@ -1113,10 +1113,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D35" s="2">
         <v>2</v>
@@ -1127,10 +1127,10 @@
         <v>5</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D36" s="2">
         <v>5</v>
@@ -1141,10 +1141,10 @@
         <v>1</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D39" s="2">
         <v>2</v>
@@ -1155,10 +1155,10 @@
         <v>2</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D40" s="2">
         <v>1</v>
@@ -1169,10 +1169,10 @@
         <v>3</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D41" s="2">
         <v>2</v>
@@ -1183,10 +1183,10 @@
         <v>4</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D42" s="2">
         <v>2</v>
@@ -1197,10 +1197,10 @@
         <v>5</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D43" s="2">
         <v>2</v>
@@ -1211,10 +1211,10 @@
         <v>6</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D44" s="2">
         <v>1</v>
@@ -1225,10 +1225,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D45" s="2">
         <v>1</v>

</xml_diff>